<commit_message>
Revert "cant save conditional"
This reverts commit c54e0609ccb60e991e7ff8f87340058f8262077b.
</commit_message>
<xml_diff>
--- a/structure_absolute.xlsx
+++ b/structure_absolute.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Desktop\Text Analysis\TextAnalysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F25CBCD-5380-454B-9FCA-F6B44CB62C20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,29 +43,29 @@
     <t>DET</t>
   </si>
   <si>
+    <t>PRON</t>
+  </si>
+  <si>
     <t>ADJ</t>
   </si>
   <si>
+    <t>ADV</t>
+  </si>
+  <si>
+    <t>CONJ</t>
+  </si>
+  <si>
+    <t>PRT</t>
+  </si>
+  <si>
     <t>NUM</t>
-  </si>
-  <si>
-    <t>ADV</t>
-  </si>
-  <si>
-    <t>CONJ</t>
-  </si>
-  <si>
-    <t>PRON</t>
-  </si>
-  <si>
-    <t>PRT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -168,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +214,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,6 +266,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,14 +459,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,141 +484,144 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.3561643835616438</v>
+        <v>0.22822729155102081</v>
       </c>
       <c r="C2">
-        <v>1586</v>
+        <v>129511</v>
       </c>
       <c r="D2">
-        <v>0.3561643835616438</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.22822729155102081</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1365371659555356</v>
+        <v>0.1921334355422801</v>
       </c>
       <c r="C3">
-        <v>608</v>
+        <v>109029</v>
       </c>
       <c r="D3">
-        <v>0.4927015495171794</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.42036072709330091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.1322703795194251</v>
+        <v>0.1288537619060206</v>
       </c>
       <c r="C4">
-        <v>589</v>
+        <v>73120</v>
       </c>
       <c r="D4">
-        <v>0.6249719290366045</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.54921448899932146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.1071187963170896</v>
+        <v>0.11694465737975029</v>
       </c>
       <c r="C5">
-        <v>477</v>
+        <v>66362</v>
       </c>
       <c r="D5">
-        <v>0.7320907253536941</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.6661591463790717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.09566584325174039</v>
+        <v>9.9458116359599266E-2</v>
       </c>
       <c r="C6">
-        <v>426</v>
+        <v>56439</v>
       </c>
       <c r="D6">
-        <v>0.8277565686054346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.76561726273867092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.04311699977543229</v>
+        <v>7.7259390446987916E-2</v>
       </c>
       <c r="C7">
-        <v>192</v>
+        <v>43842</v>
       </c>
       <c r="D7">
-        <v>0.8708735683808668</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.84287665318565885</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.03682910397484842</v>
+        <v>6.8488805476989767E-2</v>
       </c>
       <c r="C8">
-        <v>164</v>
+        <v>38865</v>
       </c>
       <c r="D8">
-        <v>0.9077026723557152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.91136545866264862</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.03503256231753873</v>
+        <v>4.2642277497290583E-2</v>
       </c>
       <c r="C9">
-        <v>156</v>
+        <v>24198</v>
       </c>
       <c r="D9">
-        <v>0.9427352346732539</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.95400773615993917</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.03054120817426454</v>
+        <v>3.5822473632735059E-2</v>
       </c>
       <c r="C10">
-        <v>136</v>
+        <v>20328</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.98983020979267422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.02672355715248147</v>
+        <v>8.9556184081837648E-3</v>
       </c>
       <c r="C11">
-        <v>119</v>
+        <v>5082</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>